<commit_message>
LAP22G31-297 #comment minor changes
</commit_message>
<xml_diff>
--- a/docs/LAPR3-2021-Self-Assessment - Sprint4.xlsx
+++ b/docs/LAPR3-2021-Self-Assessment - Sprint4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\lapr3-2021-g031\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diasd\OneDrive\Documentos\lapr3-2021-g031\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68B967FE-7F3A-4E5B-A612-2BD9E1DADFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEACD9C-66A2-40AB-AFDB-BC96DE0EFDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1493,7 +1493,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1886,7 +1886,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2186,36 +2186,36 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.8984375" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>190</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2226,13 +2226,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="86" t="s">
@@ -2254,7 +2254,7 @@
       <c r="S8" s="87"/>
       <c r="T8" s="88"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="44">
@@ -2321,7 +2321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="83" t="s">
         <v>6</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="84"/>
       <c r="C11" s="8">
         <v>1171444</v>
@@ -2383,16 +2383,26 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="84"/>
       <c r="C12" s="8">
         <v>1190539</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="8"/>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="38">
+        <v>4</v>
+      </c>
+      <c r="G12" s="37">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -2403,12 +2413,12 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="53" t="e">
+      <c r="S12" s="53">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="84"/>
       <c r="C13" s="8">
         <v>1190797</v>
@@ -2433,7 +2443,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="84"/>
       <c r="C14" s="8">
         <v>1190818</v>
@@ -2458,7 +2468,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="84"/>
       <c r="C15" s="8" t="s">
         <v>7</v>
@@ -2483,7 +2493,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="84"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
@@ -2508,7 +2518,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="84"/>
       <c r="C17" s="8" t="s">
         <v>9</v>
@@ -2533,7 +2543,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="84"/>
       <c r="C18" s="8" t="s">
         <v>10</v>
@@ -2558,7 +2568,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="84"/>
       <c r="C19" s="8" t="s">
         <v>11</v>
@@ -2583,7 +2593,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="84"/>
       <c r="C20" s="8" t="s">
         <v>12</v>
@@ -2608,7 +2618,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="84"/>
       <c r="C21" s="8" t="s">
         <v>13</v>
@@ -2633,7 +2643,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="84"/>
       <c r="C22" s="8" t="s">
         <v>14</v>
@@ -2658,7 +2668,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="84"/>
       <c r="C23" s="8" t="s">
         <v>15</v>
@@ -2683,7 +2693,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="85"/>
       <c r="C24" s="42" t="s">
         <v>16</v>
@@ -2708,7 +2718,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="47" t="s">
         <v>5</v>
@@ -2723,7 +2733,7 @@
       </c>
       <c r="F25" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="G25" s="48">
         <f t="shared" si="1"/>
@@ -2775,27 +2785,27 @@
       </c>
       <c r="S25" s="55"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2803,7 +2813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2811,7 +2821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2819,7 +2829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2835,7 +2845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2863,25 +2873,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
         <v>28</v>
       </c>
@@ -2913,7 +2923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="84"/>
       <c r="B4" s="92"/>
       <c r="C4" s="92"/>
@@ -2937,7 +2947,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="84"/>
       <c r="B5" s="92"/>
       <c r="C5" s="92"/>
@@ -2961,7 +2971,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>401</v>
       </c>
@@ -2991,7 +3001,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>402</v>
       </c>
@@ -3019,7 +3029,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="82">
         <v>403</v>
       </c>
@@ -3049,7 +3059,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="82">
         <v>404</v>
       </c>
@@ -3077,7 +3087,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="82">
         <v>405</v>
       </c>
@@ -3105,12 +3115,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="82">
         <v>406</v>
       </c>
       <c r="B11" s="30">
-        <v>1190539</v>
+        <v>1171444</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="74"/>
@@ -3133,14 +3143,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="82">
         <v>407</v>
       </c>
       <c r="B12" s="30">
-        <v>1171444</v>
-      </c>
-      <c r="C12" s="30"/>
+        <v>1190539</v>
+      </c>
+      <c r="C12" s="30">
+        <v>4</v>
+      </c>
       <c r="D12" s="74"/>
       <c r="E12" s="14" t="s">
         <v>38</v>
@@ -3161,7 +3173,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="82">
         <v>408</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="82">
         <v>409</v>
       </c>
@@ -3215,14 +3227,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="82">
         <v>410</v>
       </c>
       <c r="B15" s="30">
         <v>1190539</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="30">
+        <v>4</v>
+      </c>
       <c r="D15" s="74"/>
       <c r="E15" s="14" t="s">
         <v>38</v>
@@ -3243,7 +3257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="82">
         <v>411</v>
       </c>
@@ -3271,7 +3285,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="82">
         <v>412</v>
       </c>
@@ -3297,7 +3311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="82">
         <v>413</v>
       </c>
@@ -3323,7 +3337,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="82">
         <v>414</v>
       </c>
@@ -3349,7 +3363,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="82">
         <v>415</v>
       </c>
@@ -3375,7 +3389,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="82">
         <v>416</v>
       </c>
@@ -3401,7 +3415,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="82">
         <v>417</v>
       </c>
@@ -3431,7 +3445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="82">
         <v>418</v>
       </c>
@@ -3459,7 +3473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="82">
         <v>419</v>
       </c>
@@ -3485,7 +3499,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="82">
         <v>420</v>
       </c>
@@ -3639,19 +3653,19 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="6" width="14.875" customWidth="1"/>
+    <col min="2" max="6" width="14.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="59" t="s">
         <v>46</v>
       </c>
@@ -3671,7 +3685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
         <v>52</v>
       </c>
@@ -3692,7 +3706,7 @@
         <v>40.999999999999943</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>53</v>
       </c>
@@ -3713,7 +3727,7 @@
         <v>4.0000000000000568</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>54</v>
       </c>
@@ -3734,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>55</v>
       </c>
@@ -3755,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>56</v>
       </c>
@@ -3771,7 +3785,7 @@
         <v>14.779999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="65"/>
       <c r="B9" s="66"/>
       <c r="C9" s="66"/>
@@ -3794,28 +3808,28 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>58</v>
       </c>
@@ -3834,8 +3848,8 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>59</v>
       </c>
@@ -3936,7 +3950,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>61</v>
       </c>
@@ -4028,7 +4042,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>63</v>
       </c>
@@ -4038,7 +4052,9 @@
       <c r="C5" s="25">
         <v>5</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="25">
+        <v>5</v>
+      </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
@@ -4077,7 +4093,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>70</v>
       </c>
@@ -4087,7 +4103,9 @@
       <c r="C6" s="25">
         <v>4</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -4126,7 +4144,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>77</v>
       </c>
@@ -4136,7 +4154,9 @@
       <c r="C7" s="25">
         <v>4</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -4175,7 +4195,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>83</v>
       </c>
@@ -4185,7 +4205,9 @@
       <c r="C8" s="25">
         <v>4</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="25">
+        <v>4</v>
+      </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -4224,7 +4246,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>57</v>
       </c>
@@ -4238,7 +4260,7 @@
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>0.89189655172413751</v>
+        <v>3.5668965517241373</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
@@ -4302,7 +4324,7 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>89</v>
       </c>
@@ -4313,7 +4335,7 @@
       </c>
       <c r="D10" s="23">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>3.56758620689655</v>
+        <v>14.267586206896549</v>
       </c>
       <c r="E10" s="23">
         <f t="shared" si="2"/>
@@ -4377,7 +4399,7 @@
       <c r="Y10" s="23"/>
       <c r="Z10" s="16"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
   </sheetData>
@@ -4396,26 +4418,26 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>90</v>
       </c>
@@ -4434,7 +4456,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>59</v>
       </c>
@@ -4535,7 +4557,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>91</v>
       </c>
@@ -4545,7 +4567,9 @@
       <c r="C4" s="25">
         <v>5</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="25">
+        <v>5</v>
+      </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -4584,12 +4608,877 @@
       <c r="Y4" s="70"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
+      </c>
+      <c r="C5" s="25">
+        <v>5</v>
+      </c>
+      <c r="D5" s="25">
+        <v>5</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="69">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S5" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="T5" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="V5" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="W5" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="X5" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="15"/>
+    </row>
+    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="25">
+        <v>5</v>
+      </c>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="69">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="S6" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="T6" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="U6" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="V6" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="W6" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="X6" s="73" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y6" s="70"/>
+      <c r="Z6" s="15"/>
+    </row>
+    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="25">
+        <v>5</v>
+      </c>
+      <c r="D7" s="25">
+        <v>5</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="69">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S7" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="T7" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="U7" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="V7" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="W7" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="X7" s="73" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y7" s="70"/>
+      <c r="Z7" s="15"/>
+    </row>
+    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="25">
+        <v>5</v>
+      </c>
+      <c r="D8" s="25">
+        <v>5</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="69">
+        <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
+        <v>5</v>
+      </c>
+      <c r="S8" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="T8" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="U8" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="V8" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="W8" s="73" t="s">
+        <v>122</v>
+      </c>
+      <c r="X8" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y8" s="70"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="25">
+        <v>4</v>
+      </c>
+      <c r="D9" s="25">
+        <v>5</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="69">
+        <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
+        <v>4.5</v>
+      </c>
+      <c r="S9" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="25">
+        <v>5</v>
+      </c>
+      <c r="D10" s="25">
+        <v>5</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="69">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="S10" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="T10" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="U10" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="V10" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="W10" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="X10" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="25">
+        <v>5</v>
+      </c>
+      <c r="D11" s="25">
+        <v>5</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="69">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="S11" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="T11" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="U11" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="V11" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="W11" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="X11" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y11" s="70"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="25">
+        <v>5</v>
+      </c>
+      <c r="D12" s="25">
+        <v>5</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="69">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S12" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="T12" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="U12" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="V12" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="W12" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="X12" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y12" s="70"/>
+      <c r="Z12" s="15"/>
+    </row>
+    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="25">
+        <v>4</v>
+      </c>
+      <c r="D13" s="25">
+        <v>4</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="69">
+        <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
+        <v>4</v>
+      </c>
+      <c r="S13" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="T13" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="U13" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="V13" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="W13" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="X13" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y13" s="70"/>
+      <c r="Z13" s="15"/>
+    </row>
+    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="C14" s="25">
+        <v>5</v>
+      </c>
+      <c r="D14" s="25">
+        <v>5</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="69">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S14" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="T14" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="U14" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="V14" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="W14" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="X14" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y14" s="70"/>
+      <c r="Z14" s="15"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="18">
+        <f>SUM(B4:B14)</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
+        <v>4.8500000000000005</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
+        <v>4.8500000000000005</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="27"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="15"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23">
+        <f>C15/5*20</f>
+        <v>19.400000000000002</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
+        <v>19.400000000000002</v>
+      </c>
+      <c r="E16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="28"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14" xr:uid="{D3D36BB4-8C88-7846-9CA6-EC1FF5BDCD69}">
+      <formula1>$S$3:$X$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AEE80F-44B5-6C40-9422-A7B92010507D}">
+  <dimension ref="A1:Z15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="20">
+        <f>'Group and Self Assessment'!C10</f>
+        <v>1161605</v>
+      </c>
+      <c r="D3" s="20">
+        <f>'Group and Self Assessment'!C11</f>
+        <v>1171444</v>
+      </c>
+      <c r="E3" s="20">
+        <f>'Group and Self Assessment'!C12</f>
+        <v>1190539</v>
+      </c>
+      <c r="F3" s="20">
+        <f>'Group and Self Assessment'!C13</f>
+        <v>1190797</v>
+      </c>
+      <c r="G3" s="20">
+        <f>'Group and Self Assessment'!C14</f>
+        <v>1190818</v>
+      </c>
+      <c r="H3" s="20" t="str">
+        <f>'Group and Self Assessment'!C15</f>
+        <v>Student 6</v>
+      </c>
+      <c r="I3" s="20" t="str">
+        <f>'Group and Self Assessment'!C16</f>
+        <v>Student 7</v>
+      </c>
+      <c r="J3" s="20" t="str">
+        <f>'Group and Self Assessment'!C17</f>
+        <v>Student 8</v>
+      </c>
+      <c r="K3" s="20" t="str">
+        <f>'Group and Self Assessment'!C18</f>
+        <v>Student 9</v>
+      </c>
+      <c r="L3" s="20" t="str">
+        <f>'Group and Self Assessment'!C19</f>
+        <v>Student 10</v>
+      </c>
+      <c r="M3" s="20" t="str">
+        <f>'Group and Self Assessment'!C20</f>
+        <v>Student 11</v>
+      </c>
+      <c r="N3" s="20" t="str">
+        <f>'Group and Self Assessment'!C21</f>
+        <v>Student 12</v>
+      </c>
+      <c r="O3" s="20" t="str">
+        <f>'Group and Self Assessment'!C22</f>
+        <v>Student 13</v>
+      </c>
+      <c r="P3" s="20" t="str">
+        <f>'Group and Self Assessment'!C23</f>
+        <v>Student 14</v>
+      </c>
+      <c r="Q3" s="20" t="str">
+        <f>'Group and Self Assessment'!C24</f>
+        <v>Student 15</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="71">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="72">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="72">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="71">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="W3" s="71">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="X3" s="71">
+        <f>5</f>
+        <v>5</v>
+      </c>
+      <c r="Y3" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C4" s="25">
+        <v>5</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="69">
+        <f t="shared" ref="R4:R12" si="0">AVERAGE(C4:Q4)</f>
+        <v>5</v>
+      </c>
+      <c r="S4" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="T4" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="U4" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="V4" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="W4" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="X4" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="79"/>
+    </row>
+    <row r="5" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="17">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C5" s="25">
         <v>5</v>
@@ -4613,37 +5502,37 @@
         <v>5</v>
       </c>
       <c r="S5" s="73" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="T5" s="73" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="U5" s="73" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="V5" s="73" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="W5" s="73" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="X5" s="73" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="Y5" s="70"/>
-      <c r="Z5" s="15"/>
-    </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>105</v>
+      <c r="Z5" s="79"/>
+    </row>
+    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="76" t="s">
+        <v>162</v>
       </c>
       <c r="B6" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="C6" s="25">
-        <v>5</v>
-      </c>
-      <c r="D6" s="25"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -4659,40 +5548,40 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="69">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S6" s="73" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="T6" s="73" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="U6" s="73" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="V6" s="73" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
       <c r="W6" s="73" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="X6" s="73" t="s">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="Y6" s="70"/>
-      <c r="Z6" s="15"/>
-    </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>112</v>
+      <c r="Z6" s="79"/>
+    </row>
+    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="76" t="s">
+        <v>164</v>
       </c>
       <c r="B7" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="C7" s="25">
-        <v>5</v>
-      </c>
-      <c r="D7" s="25"/>
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -4708,40 +5597,40 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="69">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S7" s="73" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="T7" s="73" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="U7" s="73" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="V7" s="73" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="W7" s="73" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="X7" s="73" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="Y7" s="70"/>
-      <c r="Z7" s="15"/>
-    </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>118</v>
+      <c r="Z7" s="79"/>
+    </row>
+    <row r="8" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="76" t="s">
+        <v>169</v>
       </c>
       <c r="B8" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="25">
-        <v>5</v>
-      </c>
-      <c r="D8" s="25"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25">
+        <v>4</v>
+      </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -4756,847 +5645,8 @@
       <c r="P8" s="25"/>
       <c r="Q8" s="25"/>
       <c r="R8" s="69">
-        <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>5</v>
-      </c>
-      <c r="S8" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="T8" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="U8" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="V8" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="W8" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="X8" s="73" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="C9" s="25">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="69">
-        <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>4</v>
-      </c>
-      <c r="S9" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="T9" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="W9" s="73"/>
-      <c r="X9" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y9" s="70"/>
-      <c r="Z9" s="15"/>
-    </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="25">
-        <v>5</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="69">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="S10" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="T10" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="U10" s="73" t="s">
-        <v>131</v>
-      </c>
-      <c r="V10" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="W10" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="X10" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y10" s="70"/>
-      <c r="Z10" s="15"/>
-    </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C11" s="25">
-        <v>5</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="69">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="S11" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="T11" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="U11" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="V11" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="W11" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="X11" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y11" s="70"/>
-      <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C12" s="25">
-        <v>5</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="69">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="S12" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="T12" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="U12" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="V12" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="W12" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="X12" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y12" s="70"/>
-      <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C13" s="25">
-        <v>4</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="69">
-        <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>4</v>
-      </c>
-      <c r="S13" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="T13" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="U13" s="73" t="s">
-        <v>145</v>
-      </c>
-      <c r="V13" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="W13" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="X13" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y13" s="70"/>
-      <c r="Z13" s="15"/>
-    </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="C14" s="25">
-        <v>5</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="69">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="S14" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="T14" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="U14" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="V14" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="W14" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="X14" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y14" s="70"/>
-      <c r="Z14" s="15"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="18">
-        <f>SUM(B4:B14)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="7">
-        <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>4.8500000000000005</v>
-      </c>
-      <c r="D15" s="7">
-        <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="27"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="15"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23">
-        <f>C15/5*20</f>
-        <v>19.400000000000002</v>
-      </c>
-      <c r="D16" s="23">
-        <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="16"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14" xr:uid="{D3D36BB4-8C88-7846-9CA6-EC1FF5BDCD69}">
-      <formula1>$S$3:$X$3</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AEE80F-44B5-6C40-9422-A7B92010507D}">
-  <dimension ref="A1:Z15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="20">
-        <f>'Group and Self Assessment'!C10</f>
-        <v>1161605</v>
-      </c>
-      <c r="D3" s="20">
-        <f>'Group and Self Assessment'!C11</f>
-        <v>1171444</v>
-      </c>
-      <c r="E3" s="20">
-        <f>'Group and Self Assessment'!C12</f>
-        <v>1190539</v>
-      </c>
-      <c r="F3" s="20">
-        <f>'Group and Self Assessment'!C13</f>
-        <v>1190797</v>
-      </c>
-      <c r="G3" s="20">
-        <f>'Group and Self Assessment'!C14</f>
-        <v>1190818</v>
-      </c>
-      <c r="H3" s="20" t="str">
-        <f>'Group and Self Assessment'!C15</f>
-        <v>Student 6</v>
-      </c>
-      <c r="I3" s="20" t="str">
-        <f>'Group and Self Assessment'!C16</f>
-        <v>Student 7</v>
-      </c>
-      <c r="J3" s="20" t="str">
-        <f>'Group and Self Assessment'!C17</f>
-        <v>Student 8</v>
-      </c>
-      <c r="K3" s="20" t="str">
-        <f>'Group and Self Assessment'!C18</f>
-        <v>Student 9</v>
-      </c>
-      <c r="L3" s="20" t="str">
-        <f>'Group and Self Assessment'!C19</f>
-        <v>Student 10</v>
-      </c>
-      <c r="M3" s="20" t="str">
-        <f>'Group and Self Assessment'!C20</f>
-        <v>Student 11</v>
-      </c>
-      <c r="N3" s="20" t="str">
-        <f>'Group and Self Assessment'!C21</f>
-        <v>Student 12</v>
-      </c>
-      <c r="O3" s="20" t="str">
-        <f>'Group and Self Assessment'!C22</f>
-        <v>Student 13</v>
-      </c>
-      <c r="P3" s="20" t="str">
-        <f>'Group and Self Assessment'!C23</f>
-        <v>Student 14</v>
-      </c>
-      <c r="Q3" s="20" t="str">
-        <f>'Group and Self Assessment'!C24</f>
-        <v>Student 15</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="71">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="72">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="U3" s="72">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="V3" s="71">
-        <f>3</f>
-        <v>3</v>
-      </c>
-      <c r="W3" s="71">
-        <f>4</f>
-        <v>4</v>
-      </c>
-      <c r="X3" s="71">
-        <f>5</f>
-        <v>5</v>
-      </c>
-      <c r="Y3" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z3" s="78" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="17">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C4" s="25">
-        <v>5</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="69">
-        <f t="shared" ref="R4:R12" si="0">AVERAGE(C4:Q4)</f>
-        <v>5</v>
-      </c>
-      <c r="S4" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="T4" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="U4" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="V4" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="W4" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="X4" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="79"/>
-    </row>
-    <row r="5" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" s="17">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C5" s="25">
-        <v>5</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="69">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="S5" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="T5" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="U5" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="V5" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="W5" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="X5" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="79"/>
-    </row>
-    <row r="6" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="17">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="69" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="T6" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="U6" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="V6" s="73" t="s">
-        <v>155</v>
-      </c>
-      <c r="W6" s="73" t="s">
-        <v>163</v>
-      </c>
-      <c r="X6" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="79"/>
-    </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="69" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="T7" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="U7" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="V7" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="W7" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="X7" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" s="70"/>
-      <c r="Z7" s="79"/>
-    </row>
-    <row r="8" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="17">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="69" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
       </c>
       <c r="S8" s="73" t="s">
         <v>152</v>
@@ -5619,7 +5669,7 @@
       <c r="Y8" s="70"/>
       <c r="Z8" s="79"/>
     </row>
-    <row r="9" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
         <v>174</v>
       </c>
@@ -5666,7 +5716,7 @@
       <c r="Y9" s="70"/>
       <c r="Z9" s="79"/>
     </row>
-    <row r="10" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="76" t="s">
         <v>177</v>
       </c>
@@ -5713,7 +5763,7 @@
       <c r="Y10" s="70"/>
       <c r="Z10" s="79"/>
     </row>
-    <row r="11" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="76" t="s">
         <v>182</v>
       </c>
@@ -5721,7 +5771,9 @@
         <v>0.15</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="D11" s="25">
+        <v>4</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -5735,9 +5787,9 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
-      <c r="R11" s="69" t="e">
+      <c r="R11" s="69">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S11" s="73" t="s">
         <v>152</v>
@@ -5760,7 +5812,7 @@
       <c r="Y11" s="70"/>
       <c r="Z11" s="79"/>
     </row>
-    <row r="12" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="76" t="s">
         <v>186</v>
       </c>
@@ -5768,7 +5820,9 @@
         <v>0.15</v>
       </c>
       <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="D12" s="25">
+        <v>4</v>
+      </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -5782,9 +5836,9 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
       <c r="Q12" s="25"/>
-      <c r="R12" s="69" t="e">
+      <c r="R12" s="69">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S12" s="73" t="s">
         <v>152</v>
@@ -5807,7 +5861,7 @@
       <c r="Y12" s="70"/>
       <c r="Z12" s="79"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="76" t="s">
         <v>57</v>
       </c>
@@ -5821,7 +5875,7 @@
       </c>
       <c r="D13" s="81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="E13" s="81">
         <f t="shared" si="1"/>
@@ -5885,7 +5939,7 @@
       <c r="Y13" s="81"/>
       <c r="Z13" s="79"/>
     </row>
-    <row r="14" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="77" t="s">
         <v>89</v>
       </c>
@@ -5896,7 +5950,7 @@
       </c>
       <c r="D14" s="23">
         <f t="shared" ref="D14:Q14" si="2">D13/5*20</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="E14" s="23">
         <f t="shared" si="2"/>
@@ -5960,7 +6014,7 @@
       <c r="Y14" s="23"/>
       <c r="Z14" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
   </sheetData>
@@ -6159,18 +6213,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6192,6 +6246,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -6205,12 +6267,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>